<commit_message>
Update Core docstring and table creation docs
Also update the template Excel files
</commit_message>
<xml_diff>
--- a/docs/_downloads/blank_v4.xlsx
+++ b/docs/_downloads/blank_v4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rnels\Documents\GitHub\costcalc2\docs\_downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39AAAA8F-0C7C-4138-8BD0-EC765A06F9F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE279C66-4609-4AD7-A64A-70A48A02FDFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{82681B47-147F-4CCB-8555-8D6F2F79B0A9}"/>
   </bookViews>
@@ -264,7 +264,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-For solvents, express the amount as volumes relative to a certain compound. E.g 1 volume = 1 L solvent per 1 kg of SM. (Which is equal to 1 mL per 1 g, etc.) If a "Volume" is given, then the "Relative" and "Sol Recyc" columns must also be completed.</t>
+For solvents, express the amount as volumes relative to a certain compound. E.g 1 volume = 1 L solvent per 1 kg of SM. (Which is equal to 1 mL per 1 g, etc.) If a "Volume" is given, then "Density" of the compound must be provided in the Materials tab.</t>
         </r>
       </text>
     </comment>
@@ -288,59 +288,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-The fractional amount of solvent that can be expected to be recycled. E.g. "0" indicates that none of this solvent can be recycled; "1" indicates that 100% of this solvent can be recycled.</t>
+(Optional) The fractional amount of Compound that can be expected to be recycled/recovered. E.g. "0" indicates that none of this compound can be recycled; "1" indicates that 100% of this compound can be recycled.</t>
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{C439D3A4-DE93-4FC7-AC81-DEC18E39CE50}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ryan Nelson:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-For compounds that need to have their prices calculated, this column is used to indicate the "Step" where this calculation takes place. The value here must come from the "Step" column.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{4278FA27-B18E-4386-A139-7313F1E432A2}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ryan Nelson:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Operating expenses (optional). This is used to add estimated operational costs on a per step basis. These are only applicable for a reaction product, and they can be added to as many reactions as desired. </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{E4632029-8B68-45A6-8BAC-EDA9D289C2C0}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{E4632029-8B68-45A6-8BAC-EDA9D289C2C0}">
       <text>
         <r>
           <rPr>
@@ -369,7 +321,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Compound</t>
   </si>
@@ -392,38 +344,23 @@
     <t>Volumes</t>
   </si>
   <si>
-    <t>Sol Recyc</t>
+    <t>$/kg</t>
   </si>
   <si>
-    <t>OPEX</t>
-  </si>
-  <si>
-    <t>Cost step</t>
-  </si>
-  <si>
-    <t>$/kg</t>
+    <t>Recycle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -437,6 +374,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -470,15 +413,162 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="31">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -861,14 +951,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67845F94-EDDC-480D-82FE-147DEA4C2785}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="19.05078125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.05078125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.83984375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -879,50 +972,50 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4"/>
-      <c r="E3" s="1"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4"/>
-      <c r="E4" s="1"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="A6" s="4"/>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="1"/>
+      <c r="A7" s="4"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="1"/>
+      <c r="A8" s="4"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="1"/>
+      <c r="A9" s="4"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="expression" dxfId="9" priority="1">
+    <cfRule type="expression" dxfId="30" priority="1">
       <formula>NOT(ISBLANK(B2))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="2">
+    <cfRule type="expression" dxfId="29" priority="2">
       <formula>NOT(ISBLANK(A2))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -933,20 +1026,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F5EA32B-47F9-4219-8A49-366A80826A6A}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="6.26171875" customWidth="1"/>
-    <col min="2" max="2" width="21.578125" customWidth="1"/>
-    <col min="3" max="3" width="7.83984375" customWidth="1"/>
+    <col min="1" max="1" width="6.26171875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="21.578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="7.83984375" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.83984375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -960,53 +1054,43 @@
         <v>6</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A1048576">
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="7" priority="6">
       <formula>NOT(ISBLANK(B2))</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:E1048576">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="0" priority="4">
       <formula>NOT(ISBLANK(A2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>NOT(ISBLANK(A2))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="1">
+      <formula>NOT(ISBLANK(B2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C1048576">
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="4" priority="8">
       <formula>NOT(ISBLANK(D2))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="8">
+    <cfRule type="expression" dxfId="3" priority="10">
       <formula>IF(NOT(ISBLANK(B2)),AND(ISBLANK(C2:D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D1048576">
-    <cfRule type="expression" dxfId="2" priority="10">
+    <cfRule type="expression" dxfId="2" priority="12">
       <formula>NOT(ISBLANK(C2))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="11">
+    <cfRule type="expression" dxfId="1" priority="13">
       <formula>IF(NOT(ISBLANK(B2)),AND(ISBLANK(C2:D2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E1048576">
-    <cfRule type="expression" dxfId="0" priority="15">
-      <formula>NOT(ISBLANK(D2))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>